<commit_message>
update to v3.0 x carriage
</commit_message>
<xml_diff>
--- a/HyperRail/Admin/Engineering Requirements.xlsx
+++ b/HyperRail/Admin/Engineering Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorian Brusind\Documents\GitHub\PersonalProjects\HyperRail\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69538460-5A46-45AA-8258-4AEBD748D892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C6A298-D1A5-46E9-B87C-9CE409124510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2370" windowWidth="25440" windowHeight="15390" xr2:uid="{E8630FD7-9DDB-417D-B105-C29E41DFA19B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8630FD7-9DDB-417D-B105-C29E41DFA19B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Customer Requirement</t>
   </si>
@@ -51,12 +51,6 @@
     <t>The system should be accurate.</t>
   </si>
   <si>
-    <t>The system should correctly count the microbial count with &gt;=90% accuracy.</t>
-  </si>
-  <si>
-    <t>The team will test and verify several samples by hand to compare to automated results</t>
-  </si>
-  <si>
     <t>The system should be safe.</t>
   </si>
   <si>
@@ -121,6 +115,15 @@
   </si>
   <si>
     <t>The system will operate will start up and shut down at varying increments of time</t>
+  </si>
+  <si>
+    <t>The system should be accurate to within +- 1% workable area</t>
+  </si>
+  <si>
+    <t>The system should be autonomous (no human intervention)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least for 8 hours (TODO - Look up official time periods for automation) </t>
   </si>
 </sst>
 </file>
@@ -327,25 +330,6 @@
   <dxfs count="9">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -468,6 +452,55 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -502,36 +535,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -546,13 +549,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55D1D1F4-4CAD-4F6A-829B-89FF5CBC16AF}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:D9" xr:uid="{55D1D1F4-4CAD-4F6A-829B-89FF5CBC16AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55D1D1F4-4CAD-4F6A-829B-89FF5CBC16AF}" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D10" xr:uid="{55D1D1F4-4CAD-4F6A-829B-89FF5CBC16AF}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4014158B-4AF3-4D4C-9525-3D7AB74916B0}" name="Customer Requirement" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{089B24B1-8BE4-4C13-BBA8-E0A1E8AA0492}" name="Engineering Requirement" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{021BCAEE-8024-416E-B6F0-68E0C396E260}" name="Verification Process" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{18AD4B5D-E7BD-4FBF-8108-9538039862B6}" name="Verification Method" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{4014158B-4AF3-4D4C-9525-3D7AB74916B0}" name="Customer Requirement" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{089B24B1-8BE4-4C13-BBA8-E0A1E8AA0492}" name="Engineering Requirement" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{021BCAEE-8024-416E-B6F0-68E0C396E260}" name="Verification Process" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{18AD4B5D-E7BD-4FBF-8108-9538039862B6}" name="Verification Method" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -855,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33941251-6DF4-43EB-A668-5EE09C11FAC0}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,113 +886,121 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>6</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C2" s="6"/>
       <c r="D2" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="D6" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="D7" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="57" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>26</v>
-      </c>
       <c r="D8" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update tape layer and more accurate pulley
</commit_message>
<xml_diff>
--- a/HyperRail/Admin/Engineering Requirements.xlsx
+++ b/HyperRail/Admin/Engineering Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorian Brusind\Documents\GitHub\PersonalProjects\HyperRail\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C6A298-D1A5-46E9-B87C-9CE409124510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EEF393-41A3-4A85-ADE3-CF9DAE52306F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8630FD7-9DDB-417D-B105-C29E41DFA19B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Customer Requirement</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t xml:space="preserve">At least for 8 hours (TODO - Look up official time periods for automation) </t>
+  </si>
+  <si>
+    <t>The system will retrieve images of its workspace</t>
+  </si>
+  <si>
+    <t>The system will produce photographs within a specified work area</t>
+  </si>
+  <si>
+    <t>The system will have a user interface</t>
+  </si>
+  <si>
+    <t>The system will accept user commands through a recognizable interface system</t>
   </si>
 </sst>
 </file>
@@ -549,8 +561,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55D1D1F4-4CAD-4F6A-829B-89FF5CBC16AF}" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:D10" xr:uid="{55D1D1F4-4CAD-4F6A-829B-89FF5CBC16AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55D1D1F4-4CAD-4F6A-829B-89FF5CBC16AF}" name="Table1" displayName="Table1" ref="A1:D12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D12" xr:uid="{55D1D1F4-4CAD-4F6A-829B-89FF5CBC16AF}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4014158B-4AF3-4D4C-9525-3D7AB74916B0}" name="Customer Requirement" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{089B24B1-8BE4-4C13-BBA8-E0A1E8AA0492}" name="Engineering Requirement" dataDxfId="2"/>
@@ -858,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33941251-6DF4-43EB-A668-5EE09C11FAC0}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,6 +1014,26 @@
       <c r="C10" s="9"/>
       <c r="D10" s="11"/>
     </row>
+    <row r="11" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update requirements and models
</commit_message>
<xml_diff>
--- a/HyperRail/Admin/Engineering Requirements.xlsx
+++ b/HyperRail/Admin/Engineering Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorian Brusind\Documents\GitHub\PersonalProjects\HyperRail\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EEF393-41A3-4A85-ADE3-CF9DAE52306F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D8E29D-0244-40EC-A1FE-16831868D871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8630FD7-9DDB-417D-B105-C29E41DFA19B}"/>
+    <workbookView xWindow="28680" yWindow="-2370" windowWidth="25440" windowHeight="15390" xr2:uid="{E8630FD7-9DDB-417D-B105-C29E41DFA19B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>Customer Requirement</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>The system can operate on standard electricity</t>
-  </si>
-  <si>
     <t xml:space="preserve">An electrical inspection will be preformed showing operation at 120V 60Hz </t>
   </si>
   <si>
@@ -114,28 +111,67 @@
     <t>The system should be reliable</t>
   </si>
   <si>
-    <t>The system will operate will start up and shut down at varying increments of time</t>
-  </si>
-  <si>
-    <t>The system should be accurate to within +- 1% workable area</t>
-  </si>
-  <si>
-    <t>The system should be autonomous (no human intervention)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At least for 8 hours (TODO - Look up official time periods for automation) </t>
-  </si>
-  <si>
-    <t>The system will retrieve images of its workspace</t>
-  </si>
-  <si>
-    <t>The system will produce photographs within a specified work area</t>
-  </si>
-  <si>
     <t>The system will have a user interface</t>
   </si>
   <si>
-    <t>The system will accept user commands through a recognizable interface system</t>
+    <t xml:space="preserve">The system should be autonomous </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system will operate normally with no human intervention for 2 hours </t>
+  </si>
+  <si>
+    <t>The system will provide visual feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system will capture images of the available workspace </t>
+  </si>
+  <si>
+    <t>The system will accept user commands through an interface system</t>
+  </si>
+  <si>
+    <t>The system should be accurate to within +- 1% of the workable area</t>
+  </si>
+  <si>
+    <t>The system will operate on US standard electricity</t>
+  </si>
+  <si>
+    <t>The system should collect data about its environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system will allow for data sampling of environmental factors (TBD) at a rate of 5Hz </t>
+  </si>
+  <si>
+    <t>The system should make data accessible</t>
+  </si>
+  <si>
+    <t>The system will make collected data available in a standard format</t>
+  </si>
+  <si>
+    <t>Human accessible electrical inputs will be properly rated for the Human Body Model ESD per JS 001</t>
+  </si>
+  <si>
+    <t>The system should have an emergency shutoff</t>
+  </si>
+  <si>
+    <t>The system will have a single contact to denergize within 1s of interaction</t>
+  </si>
+  <si>
+    <t>A 100pf Capactior in series with a 1500Ohm resistor will be charged to 2kV and will be discharged to the defined accessible inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system will operate continueously for a minimum of 6 hours  </t>
+  </si>
+  <si>
+    <t>The System will use commercially available cabling</t>
+  </si>
+  <si>
+    <t>The system will utilize cabling solutions that can be purchased at nearby hardware stores</t>
+  </si>
+  <si>
+    <t>The system will use standard structual materials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system mechanical assembly will contain a minimum of 50% COTS parts by number </t>
   </si>
 </sst>
 </file>
@@ -561,8 +597,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55D1D1F4-4CAD-4F6A-829B-89FF5CBC16AF}" name="Table1" displayName="Table1" ref="A1:D12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:D12" xr:uid="{55D1D1F4-4CAD-4F6A-829B-89FF5CBC16AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55D1D1F4-4CAD-4F6A-829B-89FF5CBC16AF}" name="Table1" displayName="Table1" ref="A1:D18" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D18" xr:uid="{55D1D1F4-4CAD-4F6A-829B-89FF5CBC16AF}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4014158B-4AF3-4D4C-9525-3D7AB74916B0}" name="Customer Requirement" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{089B24B1-8BE4-4C13-BBA8-E0A1E8AA0492}" name="Engineering Requirement" dataDxfId="2"/>
@@ -870,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33941251-6DF4-43EB-A668-5EE09C11FAC0}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +939,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7" t="s">
@@ -926,13 +962,13 @@
     </row>
     <row r="4" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>8</v>
@@ -940,13 +976,13 @@
     </row>
     <row r="5" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>8</v>
@@ -954,13 +990,13 @@
     </row>
     <row r="6" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>9</v>
@@ -968,13 +1004,13 @@
     </row>
     <row r="7" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>8</v>
@@ -982,57 +1018,119 @@
     </row>
     <row r="8" spans="1:4" ht="57" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>24</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="11"/>
+    </row>
+    <row r="13" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="1:4" ht="57" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="11"/>
+    </row>
+    <row r="16" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>